<commit_message>
more data and png files
</commit_message>
<xml_diff>
--- a/report/Approaches_Compare_Table.xlsx
+++ b/report/Approaches_Compare_Table.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pe.li/git/Stanford_CS234_RL/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pe.li/git/stock/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F8C082-1756-864B-A55B-2036B7DC638F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C307B5-06E5-C94B-A651-345DD739A9CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="1980" windowWidth="18020" windowHeight="10440" xr2:uid="{92D66643-755B-944B-93EF-F3FB225F5D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Alg</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Yearly Return</t>
+  </si>
+  <si>
+    <t>PPO2</t>
   </si>
 </sst>
 </file>
@@ -83,9 +86,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,14 +97,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -134,9 +129,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D379685D-6A7F-AD49-96FA-63EC6F8F413E}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,7 +513,7 @@
       <c r="F2" s="1">
         <v>17067.598630781766</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <f>(F2-10000)/10000 * (365/K1)</f>
         <v>0.22334835499873115</v>
       </c>
@@ -545,7 +540,7 @@
       <c r="F3" s="1">
         <v>17352.436973246822</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <f>(F3-10000)/10000 * (365/K1)</f>
         <v>0.23234973984719395</v>
       </c>
@@ -572,8 +567,8 @@
       <c r="F4" s="1">
         <v>17516.571684288661</v>
       </c>
-      <c r="H4" s="4">
-        <f t="shared" ref="H3:H11" si="0">(F4-10000)/10000 * (365/K3)</f>
+      <c r="H4" s="3">
+        <f t="shared" ref="H4:H11" si="0">(F4-10000)/10000 * (365/K3)</f>
         <v>0.23753668093206592</v>
       </c>
       <c r="K4">
@@ -599,7 +594,7 @@
       <c r="F5" s="1">
         <v>17277.205051042754</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>0.22997228083381865</v>
       </c>
@@ -626,7 +621,7 @@
       <c r="F6" s="1">
         <v>16678.47477790351</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f t="shared" si="0"/>
         <v>0.21105136744024078</v>
       </c>
@@ -653,7 +648,7 @@
       <c r="F7" s="1">
         <v>17583.996316816356</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f t="shared" si="0"/>
         <v>0.23966741607255151</v>
       </c>
@@ -683,7 +678,7 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <f t="shared" si="0"/>
         <v>0.21564808516563769</v>
       </c>
@@ -710,7 +705,7 @@
       <c r="F9" s="1">
         <v>16899.820188736398</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <f t="shared" si="0"/>
         <v>0.21804626570465674</v>
       </c>
@@ -737,7 +732,7 @@
       <c r="F10" s="1">
         <v>16819.739137698252</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <f t="shared" si="0"/>
         <v>0.21551556582336467</v>
       </c>
@@ -746,15 +741,27 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3">
-        <v>15176.64</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14120.883959999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>21060.503959999998</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1532.224467</v>
+      </c>
+      <c r="F11" s="5">
+        <v>17096.225419999999</v>
+      </c>
+      <c r="H11" s="3">
         <f t="shared" si="0"/>
-        <v>0.16359078787878786</v>
+        <v>0.22425301110822507</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -762,9 +769,14 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="H12" s="5">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>15176.64</v>
+      </c>
+      <c r="H16" s="4">
         <f>H3-H11</f>
-        <v>6.875895196840609E-2</v>
+        <v>8.0967287389688836E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The files from Baselines
</commit_message>
<xml_diff>
--- a/report/Approaches_Compare_Table.xlsx
+++ b/report/Approaches_Compare_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pe.li/git/stock/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C307B5-06E5-C94B-A651-345DD739A9CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743AA72F-8AFD-1E41-809F-F40CDEAF2F48}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="1980" windowWidth="18020" windowHeight="10440" xr2:uid="{92D66643-755B-944B-93EF-F3FB225F5D8D}"/>
+    <workbookView xWindow="1500" yWindow="1980" windowWidth="18020" windowHeight="10440" xr2:uid="{92D66643-755B-944B-93EF-F3FB225F5D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Alg</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>PPO2</t>
+  </si>
+  <si>
+    <t>PRIVE+VOL</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C11" sqref="C11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,27 +751,41 @@
         <v>7</v>
       </c>
       <c r="C11" s="1">
-        <v>14120.883959999999</v>
+        <v>14890.763749387301</v>
       </c>
       <c r="D11" s="1">
-        <v>21060.503959999998</v>
+        <v>22335.029821411099</v>
       </c>
       <c r="E11" s="1">
-        <v>1532.224467</v>
+        <v>1279.6239764917827</v>
       </c>
       <c r="F11" s="5">
-        <v>17096.225419999999</v>
+        <v>17112.929523077662</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="0"/>
-        <v>0.22425301110822507</v>
+        <v>0.22478088969033305</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1">
+        <v>13963.501355182199</v>
+      </c>
+      <c r="D12" s="1">
+        <v>21294.655943123598</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1295.9528501222114</v>
+      </c>
+      <c r="F12" s="1">
+        <v>16826.283226245319</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F16">
@@ -776,7 +793,7 @@
       </c>
       <c r="H16" s="4">
         <f>H3-H11</f>
-        <v>8.0967287389688836E-3</v>
+        <v>7.5688501568609012E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>